<commit_message>
Add keywords management (admin) + split keywords' cat & tag
</commit_message>
<xml_diff>
--- a/config/data_keywords.xlsx
+++ b/config/data_keywords.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Stage\Referencement-Microscopes-ReMiSoL\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F10368D-6BAC-45A3-9792-8A1DF97F7B56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCC965BE-D2DD-4057-8BDF-2CC6B8DBC47D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0E5F2783-0881-4071-B044-90982E8746C1}"/>
+    <workbookView xWindow="765" yWindow="16980" windowWidth="21600" windowHeight="11295" xr2:uid="{0E5F2783-0881-4071-B044-90982E8746C1}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -531,7 +531,7 @@
   <dimension ref="A1:F43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D43"/>
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -539,7 +539,8 @@
     <col min="1" max="1" width="4.5703125" customWidth="1"/>
     <col min="2" max="2" width="21.85546875" customWidth="1"/>
     <col min="3" max="3" width="29.5703125" customWidth="1"/>
-    <col min="4" max="4" width="65.7109375" customWidth="1"/>
+    <col min="4" max="4" width="37.5703125" customWidth="1"/>
+    <col min="5" max="5" width="65.7109375" customWidth="1"/>
     <col min="6" max="6" width="32.140625" customWidth="1"/>
     <col min="8" max="8" width="48.28515625" customWidth="1"/>
     <col min="9" max="9" width="63.140625" customWidth="1"/>
@@ -558,8 +559,12 @@
         <v>0</v>
       </c>
       <c r="D1" t="str">
-        <f>"insert into keyword values("&amp;ROW()&amp;",'"&amp;B1&amp;"','"&amp;REPLACE(C1,1,1,UPPER(LEFT(C1,1)))&amp;"');"</f>
-        <v>insert into keyword values(1,'Environnement','Milieu liquide');</v>
+        <f>"insert into category values(NULL, '"&amp;B1&amp;"');"</f>
+        <v>insert into category values(NULL, 'Environnement');</v>
+      </c>
+      <c r="E1" t="str">
+        <f>"insert into keyword values("&amp;ROW()&amp;",1,'"&amp;REPLACE(C1,1,1,UPPER(LEFT(C1,1)))&amp;"');"</f>
+        <v>insert into keyword values(1,1,'Milieu liquide');</v>
       </c>
       <c r="F1" t="e">
         <f>"insert into controller values("&amp;B6&amp;", '"&amp;#REF!&amp;"',"&amp;$G$2&amp;");"</f>
@@ -576,9 +581,9 @@
       <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" t="str">
-        <f t="shared" ref="D2:D43" si="0">"insert into keyword values("&amp;ROW()&amp;",'"&amp;B2&amp;"','"&amp;REPLACE(C2,1,1,UPPER(LEFT(C2,1)))&amp;"');"</f>
-        <v>insert into keyword values(2,'Environnement','Ultravide');</v>
+      <c r="E2" t="str">
+        <f t="shared" ref="E2:E5" si="0">"insert into keyword values("&amp;ROW()&amp;",1,'"&amp;REPLACE(C2,1,1,UPPER(LEFT(C2,1)))&amp;"');"</f>
+        <v>insert into keyword values(2,1,'Ultravide');</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -591,9 +596,9 @@
       <c r="C3" t="s">
         <v>11</v>
       </c>
-      <c r="D3" t="str">
+      <c r="E3" t="str">
         <f t="shared" si="0"/>
-        <v>insert into keyword values(3,'Environnement','Vide');</v>
+        <v>insert into keyword values(3,1,'Vide');</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -606,9 +611,9 @@
       <c r="C4" t="s">
         <v>15</v>
       </c>
-      <c r="D4" t="str">
+      <c r="E4" t="str">
         <f t="shared" si="0"/>
-        <v>insert into keyword values(4,'Environnement','Air');</v>
+        <v>insert into keyword values(4,1,'Air');</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -621,9 +626,9 @@
       <c r="C5" t="s">
         <v>19</v>
       </c>
-      <c r="D5" t="str">
+      <c r="E5" t="str">
         <f t="shared" si="0"/>
-        <v>insert into keyword values(5,'Environnement','Atmosphère contrôlée');</v>
+        <v>insert into keyword values(5,1,'Atmosphère contrôlée');</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -637,8 +642,12 @@
         <v>1</v>
       </c>
       <c r="D6" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into keyword values(6,'Modes','Contact');</v>
+        <f>"insert into category values(NULL, '"&amp;B6&amp;"');"</f>
+        <v>insert into category values(NULL, 'Modes');</v>
+      </c>
+      <c r="E6" t="str">
+        <f>"insert into keyword values("&amp;ROW()&amp;",2,'"&amp;REPLACE(C6,1,1,UPPER(LEFT(C6,1)))&amp;"');"</f>
+        <v>insert into keyword values(6,2,'Contact');</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -651,9 +660,9 @@
       <c r="C7" t="s">
         <v>5</v>
       </c>
-      <c r="D7" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into keyword values(7,'Modes','Tapping');</v>
+      <c r="E7" t="str">
+        <f t="shared" ref="E7:E25" si="1">"insert into keyword values("&amp;ROW()&amp;",2,'"&amp;REPLACE(C7,1,1,UPPER(LEFT(C7,1)))&amp;"');"</f>
+        <v>insert into keyword values(7,2,'Tapping');</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -666,9 +675,9 @@
       <c r="C8" t="s">
         <v>8</v>
       </c>
-      <c r="D8" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into keyword values(8,'Modes','Non contact');</v>
+      <c r="E8" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into keyword values(8,2,'Non contact');</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -681,9 +690,9 @@
       <c r="C9" t="s">
         <v>12</v>
       </c>
-      <c r="D9" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into keyword values(9,'Modes','Spectroscopie');</v>
+      <c r="E9" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into keyword values(9,2,'Spectroscopie');</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -696,9 +705,9 @@
       <c r="C10" t="s">
         <v>16</v>
       </c>
-      <c r="D10" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into keyword values(10,'Modes','Q+');</v>
+      <c r="E10" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into keyword values(10,2,'Q+');</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -711,9 +720,9 @@
       <c r="C11" t="s">
         <v>20</v>
       </c>
-      <c r="D11" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into keyword values(11,'Modes','SCM');</v>
+      <c r="E11" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into keyword values(11,2,'SCM');</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -726,9 +735,9 @@
       <c r="C12" t="s">
         <v>23</v>
       </c>
-      <c r="D12" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into keyword values(12,'Modes','SSRM');</v>
+      <c r="E12" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into keyword values(12,2,'SSRM');</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -741,9 +750,9 @@
       <c r="C13" t="s">
         <v>26</v>
       </c>
-      <c r="D13" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into keyword values(13,'Modes','CAFM');</v>
+      <c r="E13" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into keyword values(13,2,'CAFM');</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -756,9 +765,9 @@
       <c r="C14" t="s">
         <v>29</v>
       </c>
-      <c r="D14" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into keyword values(14,'Modes','SThM');</v>
+      <c r="E14" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into keyword values(14,2,'SThM');</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -771,9 +780,9 @@
       <c r="C15" t="s">
         <v>32</v>
       </c>
-      <c r="D15" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into keyword values(15,'Modes','KPFM');</v>
+      <c r="E15" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into keyword values(15,2,'KPFM');</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -786,12 +795,12 @@
       <c r="C16" t="s">
         <v>33</v>
       </c>
-      <c r="D16" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into keyword values(16,'Modes','EFM');</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E16" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into keyword values(16,2,'EFM');</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>17</v>
       </c>
@@ -801,12 +810,12 @@
       <c r="C17" t="s">
         <v>34</v>
       </c>
-      <c r="D17" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into keyword values(17,'Modes','PFAFM');</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E17" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into keyword values(17,2,'PFAFM');</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>18</v>
       </c>
@@ -816,12 +825,12 @@
       <c r="C18" t="s">
         <v>35</v>
       </c>
-      <c r="D18" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into keyword values(18,'Modes','FluidFM');</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E18" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into keyword values(18,2,'FluidFM');</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>19</v>
       </c>
@@ -831,12 +840,12 @@
       <c r="C19" t="s">
         <v>36</v>
       </c>
-      <c r="D19" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into keyword values(19,'Modes','PFM');</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E19" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into keyword values(19,2,'PFM');</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>20</v>
       </c>
@@ -846,12 +855,12 @@
       <c r="C20" t="s">
         <v>37</v>
       </c>
-      <c r="D20" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into keyword values(20,'Modes','Nanoindentation');</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E20" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into keyword values(20,2,'Nanoindentation');</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>21</v>
       </c>
@@ -861,12 +870,12 @@
       <c r="C21" t="s">
         <v>38</v>
       </c>
-      <c r="D21" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into keyword values(21,'Modes','Nanolithographie');</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E21" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into keyword values(21,2,'Nanolithographie');</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>22</v>
       </c>
@@ -876,12 +885,12 @@
       <c r="C22" t="s">
         <v>39</v>
       </c>
-      <c r="D22" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into keyword values(22,'Modes','Nanomanipulation');</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E22" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into keyword values(22,2,'Nanomanipulation');</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>23</v>
       </c>
@@ -891,12 +900,12 @@
       <c r="C23" t="s">
         <v>40</v>
       </c>
-      <c r="D23" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into keyword values(23,'Modes','LFM');</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E23" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into keyword values(23,2,'LFM');</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>24</v>
       </c>
@@ -906,12 +915,12 @@
       <c r="C24" t="s">
         <v>41</v>
       </c>
-      <c r="D24" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into keyword values(24,'Modes','MFM');</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E24" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into keyword values(24,2,'MFM');</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>25</v>
       </c>
@@ -921,12 +930,12 @@
       <c r="C25" t="s">
         <v>42</v>
       </c>
-      <c r="D25" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into keyword values(25,'Modes','STM');</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E25" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into keyword values(25,2,'STM');</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>26</v>
       </c>
@@ -937,11 +946,15 @@
         <v>2</v>
       </c>
       <c r="D26" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into keyword values(26,'Matériaux','Oxydes');</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+        <f>"insert into category values(NULL, '"&amp;B26&amp;"');"</f>
+        <v>insert into category values(NULL, 'Matériaux');</v>
+      </c>
+      <c r="E26" t="str">
+        <f>"insert into keyword values("&amp;ROW()&amp;",3,'"&amp;REPLACE(C26,1,1,UPPER(LEFT(C26,1)))&amp;"');"</f>
+        <v>insert into keyword values(26,3,'Oxydes');</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>27</v>
       </c>
@@ -951,12 +964,12 @@
       <c r="C27" t="s">
         <v>6</v>
       </c>
-      <c r="D27" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into keyword values(27,'Matériaux','Métaux');</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E27" t="str">
+        <f t="shared" ref="E27:E34" si="2">"insert into keyword values("&amp;ROW()&amp;",3,'"&amp;REPLACE(C27,1,1,UPPER(LEFT(C27,1)))&amp;"');"</f>
+        <v>insert into keyword values(27,3,'Métaux');</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>28</v>
       </c>
@@ -966,12 +979,12 @@
       <c r="C28" t="s">
         <v>9</v>
       </c>
-      <c r="D28" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into keyword values(28,'Matériaux','Polymère');</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E28" t="str">
+        <f t="shared" si="2"/>
+        <v>insert into keyword values(28,3,'Polymère');</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>29</v>
       </c>
@@ -981,12 +994,12 @@
       <c r="C29" t="s">
         <v>13</v>
       </c>
-      <c r="D29" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into keyword values(29,'Matériaux','Minéraux');</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E29" t="str">
+        <f t="shared" si="2"/>
+        <v>insert into keyword values(29,3,'Minéraux');</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>30</v>
       </c>
@@ -996,12 +1009,12 @@
       <c r="C30" t="s">
         <v>17</v>
       </c>
-      <c r="D30" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into keyword values(30,'Matériaux','Molécule');</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E30" t="str">
+        <f t="shared" si="2"/>
+        <v>insert into keyword values(30,3,'Molécule');</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>31</v>
       </c>
@@ -1011,12 +1024,12 @@
       <c r="C31" t="s">
         <v>21</v>
       </c>
-      <c r="D31" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into keyword values(31,'Matériaux','Graphène');</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E31" t="str">
+        <f t="shared" si="2"/>
+        <v>insert into keyword values(31,3,'Graphène');</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>32</v>
       </c>
@@ -1026,12 +1039,12 @@
       <c r="C32" t="s">
         <v>24</v>
       </c>
-      <c r="D32" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into keyword values(32,'Matériaux','Bois');</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E32" t="str">
+        <f t="shared" si="2"/>
+        <v>insert into keyword values(32,3,'Bois');</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>33</v>
       </c>
@@ -1041,12 +1054,12 @@
       <c r="C33" t="s">
         <v>27</v>
       </c>
-      <c r="D33" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into keyword values(33,'Matériaux','Semi-conducteur');</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E33" t="str">
+        <f t="shared" si="2"/>
+        <v>insert into keyword values(33,3,'Semi-conducteur');</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>34</v>
       </c>
@@ -1056,12 +1069,12 @@
       <c r="C34" t="s">
         <v>30</v>
       </c>
-      <c r="D34" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into keyword values(34,'Matériaux','Organique');</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E34" t="str">
+        <f t="shared" si="2"/>
+        <v>insert into keyword values(34,3,'Organique');</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>35</v>
       </c>
@@ -1072,11 +1085,15 @@
         <v>3</v>
       </c>
       <c r="D35" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into keyword values(35,'Thématiques','Biologie');</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+        <f>"insert into category values(NULL, '"&amp;B35&amp;"');"</f>
+        <v>insert into category values(NULL, 'Thématiques');</v>
+      </c>
+      <c r="E35" t="str">
+        <f>"insert into keyword values("&amp;ROW()&amp;",4,'"&amp;REPLACE(C35,1,1,UPPER(LEFT(C35,1)))&amp;"');"</f>
+        <v>insert into keyword values(35,4,'Biologie');</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>36</v>
       </c>
@@ -1086,12 +1103,12 @@
       <c r="C36" t="s">
         <v>7</v>
       </c>
-      <c r="D36" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into keyword values(36,'Thématiques','Matériaux mous');</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E36" t="str">
+        <f t="shared" ref="E36:E43" si="3">"insert into keyword values("&amp;ROW()&amp;",4,'"&amp;REPLACE(C36,1,1,UPPER(LEFT(C36,1)))&amp;"');"</f>
+        <v>insert into keyword values(36,4,'Matériaux mous');</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>37</v>
       </c>
@@ -1101,12 +1118,12 @@
       <c r="C37" t="s">
         <v>10</v>
       </c>
-      <c r="D37" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into keyword values(37,'Thématiques','Rhéologie');</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E37" t="str">
+        <f t="shared" si="3"/>
+        <v>insert into keyword values(37,4,'Rhéologie');</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>38</v>
       </c>
@@ -1116,12 +1133,12 @@
       <c r="C38" t="s">
         <v>14</v>
       </c>
-      <c r="D38" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into keyword values(38,'Thématiques','Magnétisme');</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E38" t="str">
+        <f t="shared" si="3"/>
+        <v>insert into keyword values(38,4,'Magnétisme');</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>39</v>
       </c>
@@ -1131,12 +1148,12 @@
       <c r="C39" t="s">
         <v>18</v>
       </c>
-      <c r="D39" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into keyword values(39,'Thématiques','Couches minces');</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E39" t="str">
+        <f t="shared" si="3"/>
+        <v>insert into keyword values(39,4,'Couches minces');</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>40</v>
       </c>
@@ -1146,12 +1163,12 @@
       <c r="C40" t="s">
         <v>22</v>
       </c>
-      <c r="D40" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into keyword values(40,'Thématiques','Autoorganisation');</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E40" t="str">
+        <f t="shared" si="3"/>
+        <v>insert into keyword values(40,4,'Autoorganisation');</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>41</v>
       </c>
@@ -1161,12 +1178,12 @@
       <c r="C41" t="s">
         <v>25</v>
       </c>
-      <c r="D41" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into keyword values(41,'Thématiques','Basse température');</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E41" t="str">
+        <f t="shared" si="3"/>
+        <v>insert into keyword values(41,4,'Basse température');</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>42</v>
       </c>
@@ -1176,12 +1193,12 @@
       <c r="C42" t="s">
         <v>28</v>
       </c>
-      <c r="D42" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into keyword values(42,'Thématiques','AFM rapide');</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E42" t="str">
+        <f t="shared" si="3"/>
+        <v>insert into keyword values(42,4,'AFM rapide');</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>43</v>
       </c>
@@ -1191,9 +1208,9 @@
       <c r="C43" t="s">
         <v>31</v>
       </c>
-      <c r="D43" t="str">
-        <f t="shared" si="0"/>
-        <v>insert into keyword values(43,'Thématiques','Batterie');</v>
+      <c r="E43" t="str">
+        <f t="shared" si="3"/>
+        <v>insert into keyword values(43,4,'Batterie');</v>
       </c>
     </row>
   </sheetData>

</xml_diff>